<commit_message>
add final performance table
</commit_message>
<xml_diff>
--- a/results/clustering_performance_results_formatted.xlsx
+++ b/results/clustering_performance_results_formatted.xlsx
@@ -479,7 +479,7 @@
         <v>3150</v>
       </c>
       <c r="E2" t="n">
-        <v>0.005761980999523075</v>
+        <v>0.005814844997075852</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +500,7 @@
         <v>2367</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006190222997247474</v>
+        <v>0.006367532994772773</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         <v>2175</v>
       </c>
       <c r="E4" t="n">
-        <v>0.006511963001685217</v>
+        <v>0.00664409499586327</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +542,7 @@
         <v>2368</v>
       </c>
       <c r="E5" t="n">
-        <v>0.007604035999975167</v>
+        <v>0.007832045004761312</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         <v>2176</v>
       </c>
       <c r="E6" t="n">
-        <v>0.007512935997510795</v>
+        <v>0.007719308996456675</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>30000</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04730153600030462</v>
+        <v>0.04857666199677624</v>
       </c>
     </row>
     <row r="8">
@@ -605,7 +605,7 @@
         <v>6178</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02572387300097034</v>
+        <v>0.02667929999734042</v>
       </c>
     </row>
     <row r="9">
@@ -626,7 +626,7 @@
         <v>4847</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02408567699967534</v>
+        <v>0.02356760600378038</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>6273</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03384470799937844</v>
+        <v>0.03446630100370385</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
         <v>4915</v>
       </c>
       <c r="E11" t="n">
-        <v>0.027853995001351</v>
+        <v>0.02830970699869795</v>
       </c>
     </row>
     <row r="12">
@@ -689,7 +689,7 @@
         <v>90000</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1383287770004245</v>
+        <v>0.1419115749959019</v>
       </c>
     </row>
     <row r="13">
@@ -710,7 +710,7 @@
         <v>17674</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1541524899985234</v>
+        <v>0.1594387959994492</v>
       </c>
     </row>
     <row r="14">
@@ -731,7 +731,7 @@
         <v>16957</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1632256230004714</v>
+        <v>0.1636550790062756</v>
       </c>
     </row>
     <row r="15">
@@ -752,7 +752,7 @@
         <v>17868</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1760726300017268</v>
+        <v>0.1818027949993848</v>
       </c>
     </row>
     <row r="16">
@@ -773,7 +773,7 @@
         <v>17071</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1711850909996429</v>
+        <v>0.173423485000967</v>
       </c>
     </row>
     <row r="17">
@@ -794,7 +794,7 @@
         <v>2136</v>
       </c>
       <c r="E17" t="n">
-        <v>0.00407123200056958</v>
+        <v>0.004217055000481196</v>
       </c>
     </row>
     <row r="18">
@@ -815,7 +815,7 @@
         <v>692</v>
       </c>
       <c r="E18" t="n">
-        <v>0.002504981999663869</v>
+        <v>0.002567946998169646</v>
       </c>
     </row>
     <row r="19">
@@ -836,7 +836,7 @@
         <v>724</v>
       </c>
       <c r="E19" t="n">
-        <v>0.002884654000808951</v>
+        <v>0.002929348993347958</v>
       </c>
     </row>
     <row r="20">
@@ -857,7 +857,7 @@
         <v>775</v>
       </c>
       <c r="E20" t="n">
-        <v>0.003398500000912463</v>
+        <v>0.003452531003858894</v>
       </c>
     </row>
     <row r="21">
@@ -878,7 +878,7 @@
         <v>794</v>
       </c>
       <c r="E21" t="n">
-        <v>0.00354360300116241</v>
+        <v>0.003682187998492736</v>
       </c>
     </row>
     <row r="22">
@@ -899,7 +899,7 @@
         <v>49840</v>
       </c>
       <c r="E22" t="n">
-        <v>0.07987784299984924</v>
+        <v>0.08219722800276941</v>
       </c>
     </row>
     <row r="23">
@@ -920,7 +920,7 @@
         <v>7851</v>
       </c>
       <c r="E23" t="n">
-        <v>0.04244323999955668</v>
+        <v>0.04459925500123063</v>
       </c>
     </row>
     <row r="24">
@@ -941,7 +941,7 @@
         <v>4784</v>
       </c>
       <c r="E24" t="n">
-        <v>0.02577765900059603</v>
+        <v>0.02536624899948947</v>
       </c>
     </row>
     <row r="25">
@@ -962,7 +962,7 @@
         <v>8319</v>
       </c>
       <c r="E25" t="n">
-        <v>0.06116665100125829</v>
+        <v>0.06241406800108962</v>
       </c>
     </row>
     <row r="26">
@@ -983,7 +983,7 @@
         <v>4809</v>
       </c>
       <c r="E26" t="n">
-        <v>0.03113197199854767</v>
+        <v>0.03140369700122392</v>
       </c>
     </row>
     <row r="27">
@@ -1004,7 +1004,7 @@
         <v>124600</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1950457220009412</v>
+        <v>0.1991850749982405</v>
       </c>
     </row>
     <row r="28">
@@ -1025,7 +1025,7 @@
         <v>20525</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1934311170007277</v>
+        <v>0.1985610080009792</v>
       </c>
     </row>
     <row r="29">
@@ -1046,7 +1046,7 @@
         <v>19504</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2007396219996735</v>
+        <v>0.1991506429985748</v>
       </c>
     </row>
     <row r="30">
@@ -1067,7 +1067,7 @@
         <v>20600</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2239625420006632</v>
+        <v>0.2231662169942865</v>
       </c>
     </row>
     <row r="31">
@@ -1088,7 +1088,7 @@
         <v>19578</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2155458359993645</v>
+        <v>0.2136441269976785</v>
       </c>
     </row>
     <row r="32">
@@ -1109,7 +1109,7 @@
         <v>2070000</v>
       </c>
       <c r="E32" t="n">
-        <v>3.548310823000065</v>
+        <v>3.625698049996572</v>
       </c>
     </row>
     <row r="33">
@@ -1130,7 +1130,7 @@
         <v>1369680</v>
       </c>
       <c r="E33" t="n">
-        <v>3.497602300001745</v>
+        <v>3.721459311003855</v>
       </c>
     </row>
     <row r="34">
@@ -1151,7 +1151,7 @@
         <v>1402847</v>
       </c>
       <c r="E34" t="n">
-        <v>4.173457550001331</v>
+        <v>4.167738889002067</v>
       </c>
     </row>
     <row r="35">
@@ -1172,7 +1172,7 @@
         <v>1605979</v>
       </c>
       <c r="E35" t="n">
-        <v>5.191319295001449</v>
+        <v>5.50981826500356</v>
       </c>
     </row>
     <row r="36">
@@ -1193,7 +1193,7 @@
         <v>1549714</v>
       </c>
       <c r="E36" t="n">
-        <v>5.300926717001857</v>
+        <v>5.514767667002161</v>
       </c>
     </row>
     <row r="37">
@@ -1214,7 +1214,7 @@
         <v>20000000</v>
       </c>
       <c r="E37" t="n">
-        <v>30.81526700599716</v>
+        <v>31.52742158600449</v>
       </c>
     </row>
     <row r="38">
@@ -1235,7 +1235,7 @@
         <v>2445462</v>
       </c>
       <c r="E38" t="n">
-        <v>12.0131396479992</v>
+        <v>12.79016619000322</v>
       </c>
     </row>
     <row r="39">
@@ -1253,10 +1253,10 @@
         <v>20</v>
       </c>
       <c r="D39" t="n">
-        <v>994530</v>
+        <v>995678</v>
       </c>
       <c r="E39" t="n">
-        <v>8.960253585999453</v>
+        <v>8.458397934999084</v>
       </c>
     </row>
     <row r="40">
@@ -1277,7 +1277,7 @@
         <v>2567188</v>
       </c>
       <c r="E40" t="n">
-        <v>22.01734304699858</v>
+        <v>23.59077057499962</v>
       </c>
     </row>
     <row r="41">
@@ -1295,10 +1295,10 @@
         <v>20</v>
       </c>
       <c r="D41" t="n">
-        <v>711514</v>
+        <v>712923</v>
       </c>
       <c r="E41" t="n">
-        <v>7.409900239999843</v>
+        <v>7.570853944998817</v>
       </c>
     </row>
     <row r="42">
@@ -1319,7 +1319,7 @@
         <v>83000000</v>
       </c>
       <c r="E42" t="n">
-        <v>125.4123725249992</v>
+        <v>128.6722444709958</v>
       </c>
     </row>
     <row r="43">
@@ -1340,7 +1340,7 @@
         <v>2734897</v>
       </c>
       <c r="E43" t="n">
-        <v>31.21775173299829</v>
+        <v>32.43403467199823</v>
       </c>
     </row>
     <row r="44">
@@ -1358,10 +1358,10 @@
         <v>100</v>
       </c>
       <c r="D44" t="n">
-        <v>1437071</v>
+        <v>1471694</v>
       </c>
       <c r="E44" t="n">
-        <v>18.15288096999939</v>
+        <v>19.53243472499889</v>
       </c>
     </row>
     <row r="45">
@@ -1382,7 +1382,7 @@
         <v>2718511</v>
       </c>
       <c r="E45" t="n">
-        <v>53.38248741600182</v>
+        <v>54.24646147800377</v>
       </c>
     </row>
     <row r="46">
@@ -1400,10 +1400,10 @@
         <v>100</v>
       </c>
       <c r="D46" t="n">
-        <v>1543909</v>
+        <v>1560019</v>
       </c>
       <c r="E46" t="n">
-        <v>29.32445465799901</v>
+        <v>28.83495225200022</v>
       </c>
     </row>
     <row r="47">
@@ -1424,7 +1424,7 @@
         <v>3690000</v>
       </c>
       <c r="E47" t="n">
-        <v>6.304882692998945</v>
+        <v>6.433731807992444</v>
       </c>
     </row>
     <row r="48">
@@ -1445,7 +1445,7 @@
         <v>2577393</v>
       </c>
       <c r="E48" t="n">
-        <v>6.472793347998959</v>
+        <v>6.76779491599882</v>
       </c>
     </row>
     <row r="49">
@@ -1463,10 +1463,10 @@
         <v>3</v>
       </c>
       <c r="D49" t="n">
-        <v>1910814</v>
+        <v>2367476</v>
       </c>
       <c r="E49" t="n">
-        <v>5.794817928999692</v>
+        <v>7.251122846995713</v>
       </c>
     </row>
     <row r="50">
@@ -1487,7 +1487,7 @@
         <v>2722276</v>
       </c>
       <c r="E50" t="n">
-        <v>8.772439460000896</v>
+        <v>9.189486382994801</v>
       </c>
     </row>
     <row r="51">
@@ -1505,10 +1505,10 @@
         <v>3</v>
       </c>
       <c r="D51" t="n">
-        <v>1957316</v>
+        <v>2420864</v>
       </c>
       <c r="E51" t="n">
-        <v>6.858587763999822</v>
+        <v>8.944107709001401</v>
       </c>
     </row>
     <row r="52">
@@ -1529,7 +1529,7 @@
         <v>16800000</v>
       </c>
       <c r="E52" t="n">
-        <v>25.89255370500177</v>
+        <v>26.43515767500503</v>
       </c>
     </row>
     <row r="53">
@@ -1550,7 +1550,7 @@
         <v>2305505</v>
       </c>
       <c r="E53" t="n">
-        <v>11.18234652200044</v>
+        <v>11.65422490199853</v>
       </c>
     </row>
     <row r="54">
@@ -1571,7 +1571,7 @@
         <v>1221798</v>
       </c>
       <c r="E54" t="n">
-        <v>9.147639416998572</v>
+        <v>8.644254487007856</v>
       </c>
     </row>
     <row r="55">
@@ -1592,7 +1592,7 @@
         <v>2479170</v>
       </c>
       <c r="E55" t="n">
-        <v>21.83810962699863</v>
+        <v>22.71688963199267</v>
       </c>
     </row>
     <row r="56">
@@ -1610,10 +1610,10 @@
         <v>20</v>
       </c>
       <c r="D56" t="n">
-        <v>1295284</v>
+        <v>1304855</v>
       </c>
       <c r="E56" t="n">
-        <v>14.23156910000034</v>
+        <v>14.8820648839901</v>
       </c>
     </row>
     <row r="57">
@@ -1634,7 +1634,7 @@
         <v>79500000</v>
       </c>
       <c r="E57" t="n">
-        <v>120.073102194001</v>
+        <v>122.2881878550106</v>
       </c>
     </row>
     <row r="58">
@@ -1655,7 +1655,7 @@
         <v>3709462</v>
       </c>
       <c r="E58" t="n">
-        <v>39.51865390799867</v>
+        <v>40.5156517590076</v>
       </c>
     </row>
     <row r="59">
@@ -1673,10 +1673,10 @@
         <v>100</v>
       </c>
       <c r="D59" t="n">
-        <v>2560489</v>
+        <v>2590602</v>
       </c>
       <c r="E59" t="n">
-        <v>38.01398573299957</v>
+        <v>35.02543567500834</v>
       </c>
     </row>
     <row r="60">
@@ -1697,7 +1697,7 @@
         <v>3641446</v>
       </c>
       <c r="E60" t="n">
-        <v>75.7583396580012</v>
+        <v>76.65954678200069</v>
       </c>
     </row>
     <row r="61">
@@ -1715,10 +1715,10 @@
         <v>100</v>
       </c>
       <c r="D61" t="n">
-        <v>2686931</v>
+        <v>2658392</v>
       </c>
       <c r="E61" t="n">
-        <v>58.93518752000091</v>
+        <v>56.02694382199843</v>
       </c>
     </row>
   </sheetData>
@@ -1785,7 +1785,7 @@
         <v>120000</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2366412209994451</v>
+        <v>0.2682985159990494</v>
       </c>
     </row>
     <row r="3">
@@ -1806,7 +1806,7 @@
         <v>148332</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3653034140006639</v>
+        <v>0.3719464620007784</v>
       </c>
     </row>
     <row r="4">
@@ -1827,7 +1827,7 @@
         <v>89398</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2606673589980346</v>
+        <v>0.2567091119999532</v>
       </c>
     </row>
     <row r="5">
@@ -1848,7 +1848,7 @@
         <v>148577</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4367120799979602</v>
+        <v>0.4515994890025468</v>
       </c>
     </row>
     <row r="6">
@@ -1869,7 +1869,7 @@
         <v>89396</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3069930739984557</v>
+        <v>0.3060872819987708</v>
       </c>
     </row>
     <row r="7">
@@ -1890,7 +1890,7 @@
         <v>13800000</v>
       </c>
       <c r="E7" t="n">
-        <v>21.72941754899875</v>
+        <v>22.69400169299479</v>
       </c>
     </row>
     <row r="8">
@@ -1911,7 +1911,7 @@
         <v>7338918</v>
       </c>
       <c r="E8" t="n">
-        <v>24.19922340599805</v>
+        <v>24.84390040899598</v>
       </c>
     </row>
     <row r="9">
@@ -1929,10 +1929,10 @@
         <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>3564179</v>
+        <v>3683702</v>
       </c>
       <c r="E9" t="n">
-        <v>19.01097077899976</v>
+        <v>18.56450153500191</v>
       </c>
     </row>
     <row r="10">
@@ -1953,7 +1953,7 @@
         <v>7379733</v>
       </c>
       <c r="E10" t="n">
-        <v>36.52100357000018</v>
+        <v>39.12159483700088</v>
       </c>
     </row>
     <row r="11">
@@ -1971,10 +1971,10 @@
         <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>3562787</v>
+        <v>3681396</v>
       </c>
       <c r="E11" t="n">
-        <v>24.59997801200007</v>
+        <v>25.59362802399846</v>
       </c>
     </row>
     <row r="12">
@@ -1995,7 +1995,7 @@
         <v>53000000</v>
       </c>
       <c r="E12" t="n">
-        <v>81.4891661340007</v>
+        <v>82.13059319600143</v>
       </c>
     </row>
     <row r="13">
@@ -2016,7 +2016,7 @@
         <v>12840348</v>
       </c>
       <c r="E13" t="n">
-        <v>53.21772702499948</v>
+        <v>54.78684354299912</v>
       </c>
     </row>
     <row r="14">
@@ -2034,10 +2034,10 @@
         <v>100</v>
       </c>
       <c r="D14" t="n">
-        <v>4399797</v>
+        <v>4577270</v>
       </c>
       <c r="E14" t="n">
-        <v>23.92198896899936</v>
+        <v>24.83796236500348</v>
       </c>
     </row>
     <row r="15">
@@ -2058,7 +2058,7 @@
         <v>12922220</v>
       </c>
       <c r="E15" t="n">
-        <v>79.32522719899862</v>
+        <v>81.11007291999704</v>
       </c>
     </row>
     <row r="16">
@@ -2076,10 +2076,10 @@
         <v>100</v>
       </c>
       <c r="D16" t="n">
-        <v>4422440</v>
+        <v>4585506</v>
       </c>
       <c r="E16" t="n">
-        <v>30.87962543599861</v>
+        <v>34.15631349700561</v>
       </c>
     </row>
     <row r="17">
@@ -2100,7 +2100,7 @@
         <v>90000</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2525308490003226</v>
+        <v>0.2705890719953459</v>
       </c>
     </row>
     <row r="18">
@@ -2121,7 +2121,7 @@
         <v>109459</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3457517669994559</v>
+        <v>0.3657100569980685</v>
       </c>
     </row>
     <row r="19">
@@ -2142,7 +2142,7 @@
         <v>94459</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3400943529995857</v>
+        <v>0.3428817160020117</v>
       </c>
     </row>
     <row r="20">
@@ -2163,7 +2163,7 @@
         <v>109459</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3849578549998114</v>
+        <v>0.4084508669984643</v>
       </c>
     </row>
     <row r="21">
@@ -2184,7 +2184,7 @@
         <v>94459</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3649997079992318</v>
+        <v>0.3937527009984478</v>
       </c>
     </row>
     <row r="22">
@@ -2205,7 +2205,7 @@
         <v>6800000</v>
       </c>
       <c r="E22" t="n">
-        <v>10.96380579499964</v>
+        <v>11.34314738299872</v>
       </c>
     </row>
     <row r="23">
@@ -2226,7 +2226,7 @@
         <v>2879836</v>
       </c>
       <c r="E23" t="n">
-        <v>10.49400146600237</v>
+        <v>11.06419250400359</v>
       </c>
     </row>
     <row r="24">
@@ -2244,10 +2244,10 @@
         <v>20</v>
       </c>
       <c r="D24" t="n">
-        <v>1653336</v>
+        <v>1810008</v>
       </c>
       <c r="E24" t="n">
-        <v>9.376761712999723</v>
+        <v>10.48195680000208</v>
       </c>
     </row>
     <row r="25">
@@ -2268,7 +2268,7 @@
         <v>2879836</v>
       </c>
       <c r="E25" t="n">
-        <v>14.95522121700196</v>
+        <v>15.38272777300153</v>
       </c>
     </row>
     <row r="26">
@@ -2286,10 +2286,10 @@
         <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>1652199</v>
+        <v>1808146</v>
       </c>
       <c r="E26" t="n">
-        <v>11.74910386099873</v>
+        <v>13.74543755099876</v>
       </c>
     </row>
     <row r="27">
@@ -2310,7 +2310,7 @@
         <v>37000000</v>
       </c>
       <c r="E27" t="n">
-        <v>58.19869944300081</v>
+        <v>59.65257723099785</v>
       </c>
     </row>
     <row r="28">
@@ -2331,7 +2331,7 @@
         <v>4972604</v>
       </c>
       <c r="E28" t="n">
-        <v>26.03568685600112</v>
+        <v>27.16683422200003</v>
       </c>
     </row>
     <row r="29">
@@ -2349,10 +2349,10 @@
         <v>100</v>
       </c>
       <c r="D29" t="n">
-        <v>3229524</v>
+        <v>3296752</v>
       </c>
       <c r="E29" t="n">
-        <v>22.84465894299865</v>
+        <v>21.95632295700489</v>
       </c>
     </row>
     <row r="30">
@@ -2373,7 +2373,7 @@
         <v>4972604</v>
       </c>
       <c r="E30" t="n">
-        <v>39.03174929799934</v>
+        <v>38.11679077900044</v>
       </c>
     </row>
     <row r="31">
@@ -2391,10 +2391,10 @@
         <v>100</v>
       </c>
       <c r="D31" t="n">
-        <v>3228516</v>
+        <v>3296222</v>
       </c>
       <c r="E31" t="n">
-        <v>26.91750436800066</v>
+        <v>26.72337685200182</v>
       </c>
     </row>
     <row r="32">
@@ -2415,7 +2415,7 @@
         <v>90000</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9202197780032293</v>
+        <v>0.9210556260004523</v>
       </c>
     </row>
     <row r="33">
@@ -2436,7 +2436,7 @@
         <v>84923</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9553866479982389</v>
+        <v>0.9796162450002157</v>
       </c>
     </row>
     <row r="34">
@@ -2457,7 +2457,7 @@
         <v>84923</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9540395519979938</v>
+        <v>0.9826084099986474</v>
       </c>
     </row>
     <row r="35">
@@ -2478,7 +2478,7 @@
         <v>84923</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9637216939991049</v>
+        <v>1.291304753001896</v>
       </c>
     </row>
     <row r="36">
@@ -2499,7 +2499,7 @@
         <v>84923</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9725447960008751</v>
+        <v>1.078869926001062</v>
       </c>
     </row>
     <row r="37">
@@ -2520,7 +2520,7 @@
         <v>6800000</v>
       </c>
       <c r="E37" t="n">
-        <v>12.40654942699985</v>
+        <v>12.85774857900105</v>
       </c>
     </row>
     <row r="38">
@@ -2541,7 +2541,7 @@
         <v>2934309</v>
       </c>
       <c r="E38" t="n">
-        <v>11.08944132199758</v>
+        <v>11.95205071999953</v>
       </c>
     </row>
     <row r="39">
@@ -2559,10 +2559,10 @@
         <v>20</v>
       </c>
       <c r="D39" t="n">
-        <v>1809460</v>
+        <v>1812148</v>
       </c>
       <c r="E39" t="n">
-        <v>9.61843961899649</v>
+        <v>8.595161565004673</v>
       </c>
     </row>
     <row r="40">
@@ -2583,7 +2583,7 @@
         <v>2934309</v>
       </c>
       <c r="E40" t="n">
-        <v>15.05070419600088</v>
+        <v>15.73497974700149</v>
       </c>
     </row>
     <row r="41">
@@ -2601,10 +2601,10 @@
         <v>20</v>
       </c>
       <c r="D41" t="n">
-        <v>1681582</v>
+        <v>1807916</v>
       </c>
       <c r="E41" t="n">
-        <v>9.828231515999505</v>
+        <v>10.92541129600431</v>
       </c>
     </row>
     <row r="42">
@@ -2625,7 +2625,7 @@
         <v>34000000</v>
       </c>
       <c r="E42" t="n">
-        <v>59.07287309000094</v>
+        <v>61.16180734999944</v>
       </c>
     </row>
     <row r="43">
@@ -2646,7 +2646,7 @@
         <v>7151322</v>
       </c>
       <c r="E43" t="n">
-        <v>39.3789760260006</v>
+        <v>41.0110633660006</v>
       </c>
     </row>
     <row r="44">
@@ -2664,10 +2664,10 @@
         <v>100</v>
       </c>
       <c r="D44" t="n">
-        <v>4091654</v>
+        <v>4236852</v>
       </c>
       <c r="E44" t="n">
-        <v>37.18949261200032</v>
+        <v>38.45806887099752</v>
       </c>
     </row>
     <row r="45">
@@ -2688,7 +2688,7 @@
         <v>7151322</v>
       </c>
       <c r="E45" t="n">
-        <v>56.30852646600033</v>
+        <v>54.65662452400284</v>
       </c>
     </row>
     <row r="46">
@@ -2706,10 +2706,10 @@
         <v>100</v>
       </c>
       <c r="D46" t="n">
-        <v>4075287</v>
+        <v>4214818</v>
       </c>
       <c r="E46" t="n">
-        <v>42.30979743100033</v>
+        <v>44.92725606800377</v>
       </c>
     </row>
     <row r="47">
@@ -2730,7 +2730,7 @@
         <v>840000</v>
       </c>
       <c r="E47" t="n">
-        <v>1.453196425998613</v>
+        <v>1.47853387700161</v>
       </c>
     </row>
     <row r="48">
@@ -2751,7 +2751,7 @@
         <v>879890</v>
       </c>
       <c r="E48" t="n">
-        <v>2.033701017997373</v>
+        <v>2.117933127010474</v>
       </c>
     </row>
     <row r="49">
@@ -2769,10 +2769,10 @@
         <v>3</v>
       </c>
       <c r="D49" t="n">
-        <v>869932</v>
+        <v>874911</v>
       </c>
       <c r="E49" t="n">
-        <v>2.304919406000408</v>
+        <v>2.330293855004129</v>
       </c>
     </row>
     <row r="50">
@@ -2793,7 +2793,7 @@
         <v>882837</v>
       </c>
       <c r="E50" t="n">
-        <v>2.560878312000568</v>
+        <v>2.702914016001159</v>
       </c>
     </row>
     <row r="51">
@@ -2811,10 +2811,10 @@
         <v>3</v>
       </c>
       <c r="D51" t="n">
-        <v>872355</v>
+        <v>877596</v>
       </c>
       <c r="E51" t="n">
-        <v>2.668313244997989</v>
+        <v>2.780574857009924</v>
       </c>
     </row>
     <row r="52">
@@ -2835,7 +2835,7 @@
         <v>6000000</v>
       </c>
       <c r="E52" t="n">
-        <v>9.350790274998872</v>
+        <v>9.504144099992118</v>
       </c>
     </row>
     <row r="53">
@@ -2856,7 +2856,7 @@
         <v>10330209</v>
       </c>
       <c r="E53" t="n">
-        <v>22.29190734900112</v>
+        <v>23.46875568499672</v>
       </c>
     </row>
     <row r="54">
@@ -2874,10 +2874,10 @@
         <v>20</v>
       </c>
       <c r="D54" t="n">
-        <v>2863457</v>
+        <v>2920537</v>
       </c>
       <c r="E54" t="n">
-        <v>7.282458959998621</v>
+        <v>7.889323527997476</v>
       </c>
     </row>
     <row r="55">
@@ -2898,7 +2898,7 @@
         <v>11052738</v>
       </c>
       <c r="E55" t="n">
-        <v>29.21839720299977</v>
+        <v>30.68521564100229</v>
       </c>
     </row>
     <row r="56">
@@ -2916,10 +2916,10 @@
         <v>20</v>
       </c>
       <c r="D56" t="n">
-        <v>2964126</v>
+        <v>3081199</v>
       </c>
       <c r="E56" t="n">
-        <v>8.681552796999313</v>
+        <v>9.229930214001797</v>
       </c>
     </row>
     <row r="57">
@@ -2940,7 +2940,7 @@
         <v>23500000</v>
       </c>
       <c r="E57" t="n">
-        <v>35.86931221099803</v>
+        <v>36.43146740799421</v>
       </c>
     </row>
     <row r="58">
@@ -2961,7 +2961,7 @@
         <v>11836355</v>
       </c>
       <c r="E58" t="n">
-        <v>30.07139873000051</v>
+        <v>31.36043068299477</v>
       </c>
     </row>
     <row r="59">
@@ -2979,10 +2979,10 @@
         <v>100</v>
       </c>
       <c r="D59" t="n">
-        <v>2284908</v>
+        <v>2541589</v>
       </c>
       <c r="E59" t="n">
-        <v>8.890125685997191</v>
+        <v>10.01124863600126</v>
       </c>
     </row>
     <row r="60">
@@ -3003,7 +3003,7 @@
         <v>20236336</v>
       </c>
       <c r="E60" t="n">
-        <v>57.93257729600009</v>
+        <v>59.77006085500761</v>
       </c>
     </row>
     <row r="61">
@@ -3021,10 +3021,10 @@
         <v>100</v>
       </c>
       <c r="D61" t="n">
-        <v>3996726</v>
+        <v>4391617</v>
       </c>
       <c r="E61" t="n">
-        <v>14.61768678500084</v>
+        <v>17.03169000300113</v>
       </c>
     </row>
     <row r="62">
@@ -3045,7 +3045,7 @@
         <v>1080000</v>
       </c>
       <c r="E62" t="n">
-        <v>1.964874081000744</v>
+        <v>2.015500535009778</v>
       </c>
     </row>
     <row r="63">
@@ -3066,7 +3066,7 @@
         <v>1110000</v>
       </c>
       <c r="E63" t="n">
-        <v>2.680567858998984</v>
+        <v>2.767837762992713</v>
       </c>
     </row>
     <row r="64">
@@ -3084,10 +3084,10 @@
         <v>3</v>
       </c>
       <c r="D64" t="n">
-        <v>1102015</v>
+        <v>1110000</v>
       </c>
       <c r="E64" t="n">
-        <v>3.018980816999829</v>
+        <v>3.048204680002527</v>
       </c>
     </row>
     <row r="65">
@@ -3108,7 +3108,7 @@
         <v>1110000</v>
       </c>
       <c r="E65" t="n">
-        <v>3.33691588000147</v>
+        <v>3.489153317001183</v>
       </c>
     </row>
     <row r="66">
@@ -3126,10 +3126,10 @@
         <v>3</v>
       </c>
       <c r="D66" t="n">
-        <v>1094784</v>
+        <v>1110000</v>
       </c>
       <c r="E66" t="n">
-        <v>3.488796052999533</v>
+        <v>3.635523675999139</v>
       </c>
     </row>
     <row r="67">
@@ -3150,7 +3150,7 @@
         <v>7900000</v>
       </c>
       <c r="E67" t="n">
-        <v>12.59128023099765</v>
+        <v>12.90621658600867</v>
       </c>
     </row>
     <row r="68">
@@ -3171,7 +3171,7 @@
         <v>3300000</v>
       </c>
       <c r="E68" t="n">
-        <v>7.222364876997744</v>
+        <v>7.472593055004836</v>
       </c>
     </row>
     <row r="69">
@@ -3189,10 +3189,10 @@
         <v>20</v>
       </c>
       <c r="D69" t="n">
-        <v>2504815</v>
+        <v>2521344</v>
       </c>
       <c r="E69" t="n">
-        <v>6.203148833999876</v>
+        <v>6.176656119001564</v>
       </c>
     </row>
     <row r="70">
@@ -3213,7 +3213,7 @@
         <v>3300000</v>
       </c>
       <c r="E70" t="n">
-        <v>8.929477404002682</v>
+        <v>9.148172245011665</v>
       </c>
     </row>
     <row r="71">
@@ -3231,10 +3231,10 @@
         <v>20</v>
       </c>
       <c r="D71" t="n">
-        <v>2146340</v>
+        <v>2197780</v>
       </c>
       <c r="E71" t="n">
-        <v>6.173867192999751</v>
+        <v>6.684663812004146</v>
       </c>
     </row>
     <row r="72">
@@ -3255,7 +3255,7 @@
         <v>9000000</v>
       </c>
       <c r="E72" t="n">
-        <v>14.03547162999894</v>
+        <v>14.33975900900259</v>
       </c>
     </row>
     <row r="73">
@@ -3276,7 +3276,7 @@
         <v>7499766</v>
       </c>
       <c r="E73" t="n">
-        <v>15.98902055600047</v>
+        <v>16.60947763400327</v>
       </c>
     </row>
     <row r="74">
@@ -3294,10 +3294,10 @@
         <v>100</v>
       </c>
       <c r="D74" t="n">
-        <v>5660515</v>
+        <v>5728941</v>
       </c>
       <c r="E74" t="n">
-        <v>14.27632354099842</v>
+        <v>14.26723371300614</v>
       </c>
     </row>
     <row r="75">
@@ -3318,7 +3318,7 @@
         <v>7499786</v>
       </c>
       <c r="E75" t="n">
-        <v>19.51649423699928</v>
+        <v>20.07715436100261</v>
       </c>
     </row>
     <row r="76">
@@ -3336,10 +3336,10 @@
         <v>100</v>
       </c>
       <c r="D76" t="n">
-        <v>4391286</v>
+        <v>4524386</v>
       </c>
       <c r="E76" t="n">
-        <v>12.88667330099997</v>
+        <v>13.50076972600073</v>
       </c>
     </row>
     <row r="77">
@@ -3360,7 +3360,7 @@
         <v>525000</v>
       </c>
       <c r="E77" t="n">
-        <v>1.353881723000086</v>
+        <v>1.361939049995271</v>
       </c>
     </row>
     <row r="78">
@@ -3381,7 +3381,7 @@
         <v>645000</v>
       </c>
       <c r="E78" t="n">
-        <v>1.976887109998643</v>
+        <v>2.023746706006932</v>
       </c>
     </row>
     <row r="79">
@@ -3402,7 +3402,7 @@
         <v>645000</v>
       </c>
       <c r="E79" t="n">
-        <v>2.173866621000343</v>
+        <v>2.18201200698968</v>
       </c>
     </row>
     <row r="80">
@@ -3423,7 +3423,7 @@
         <v>645000</v>
       </c>
       <c r="E80" t="n">
-        <v>2.349104222001188</v>
+        <v>2.435108170000603</v>
       </c>
     </row>
     <row r="81">
@@ -3444,7 +3444,7 @@
         <v>645000</v>
       </c>
       <c r="E81" t="n">
-        <v>2.426959681000881</v>
+        <v>2.522327739992761</v>
       </c>
     </row>
     <row r="82">
@@ -3465,7 +3465,7 @@
         <v>3100000</v>
       </c>
       <c r="E82" t="n">
-        <v>5.565243741002632</v>
+        <v>5.685102400006144</v>
       </c>
     </row>
     <row r="83">
@@ -3486,7 +3486,7 @@
         <v>2200000</v>
       </c>
       <c r="E83" t="n">
-        <v>5.326035953999963</v>
+        <v>5.517453352993471</v>
       </c>
     </row>
     <row r="84">
@@ -3504,10 +3504,10 @@
         <v>20</v>
       </c>
       <c r="D84" t="n">
-        <v>2130270</v>
+        <v>2009427</v>
       </c>
       <c r="E84" t="n">
-        <v>5.673971755000821</v>
+        <v>5.400286649004556</v>
       </c>
     </row>
     <row r="85">
@@ -3528,7 +3528,7 @@
         <v>2200000</v>
       </c>
       <c r="E85" t="n">
-        <v>6.492958118000388</v>
+        <v>6.815596347005339</v>
       </c>
     </row>
     <row r="86">
@@ -3546,10 +3546,10 @@
         <v>20</v>
       </c>
       <c r="D86" t="n">
-        <v>1638100</v>
+        <v>1704140</v>
       </c>
       <c r="E86" t="n">
-        <v>5.106327007997606</v>
+        <v>5.578219893999631</v>
       </c>
     </row>
     <row r="87">
@@ -3570,7 +3570,7 @@
         <v>7000000</v>
       </c>
       <c r="E87" t="n">
-        <v>11.92492063799727</v>
+        <v>12.1889516129886</v>
       </c>
     </row>
     <row r="88">
@@ -3591,7 +3591,7 @@
         <v>6934999</v>
       </c>
       <c r="E88" t="n">
-        <v>15.95513034199757</v>
+        <v>16.52494321099948</v>
       </c>
     </row>
     <row r="89">
@@ -3609,10 +3609,10 @@
         <v>100</v>
       </c>
       <c r="D89" t="n">
-        <v>6330177</v>
+        <v>6357527</v>
       </c>
       <c r="E89" t="n">
-        <v>15.89969014099916</v>
+        <v>16.0716983799939</v>
       </c>
     </row>
     <row r="90">
@@ -3633,7 +3633,7 @@
         <v>6934999</v>
       </c>
       <c r="E90" t="n">
-        <v>18.56286055500095</v>
+        <v>19.15556146799645</v>
       </c>
     </row>
     <row r="91">
@@ -3651,10 +3651,10 @@
         <v>100</v>
       </c>
       <c r="D91" t="n">
-        <v>3794620</v>
+        <v>3860059</v>
       </c>
       <c r="E91" t="n">
-        <v>11.16225960600059</v>
+        <v>11.48711841800832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final pass over the readme, add binary files for ease of use
</commit_message>
<xml_diff>
--- a/results/clustering_performance_results_formatted.xlsx
+++ b/results/clustering_performance_results_formatted.xlsx
@@ -479,7 +479,7 @@
         <v>3150</v>
       </c>
       <c r="E2" t="n">
-        <v>0.005814844997075852</v>
+        <v>0.01058877300238237</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +500,7 @@
         <v>2367</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006367532994772773</v>
+        <v>0.01084896300744731</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         <v>2175</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00664409499586327</v>
+        <v>0.0112079660029849</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +542,7 @@
         <v>2368</v>
       </c>
       <c r="E5" t="n">
-        <v>0.007832045004761312</v>
+        <v>0.01250027200148907</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         <v>2176</v>
       </c>
       <c r="E6" t="n">
-        <v>0.007719308996456675</v>
+        <v>0.01222316898929421</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>30000</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04857666199677624</v>
+        <v>0.08242858799349051</v>
       </c>
     </row>
     <row r="8">
@@ -605,7 +605,7 @@
         <v>6178</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02667929999734042</v>
+        <v>0.04035628600104246</v>
       </c>
     </row>
     <row r="9">
@@ -626,7 +626,7 @@
         <v>4847</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02356760600378038</v>
+        <v>0.03688739400240593</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>6273</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03446630100370385</v>
+        <v>0.05002444199635647</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
         <v>4915</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02830970699869795</v>
+        <v>0.04121896599826869</v>
       </c>
     </row>
     <row r="12">
@@ -689,7 +689,7 @@
         <v>90000</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1419115749959019</v>
+        <v>0.2398643740016269</v>
       </c>
     </row>
     <row r="13">
@@ -710,7 +710,7 @@
         <v>17674</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1594387959994492</v>
+        <v>0.2510825019999174</v>
       </c>
     </row>
     <row r="14">
@@ -731,7 +731,7 @@
         <v>16957</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1636550790062756</v>
+        <v>0.2618665240006521</v>
       </c>
     </row>
     <row r="15">
@@ -752,7 +752,7 @@
         <v>17868</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1818027949993848</v>
+        <v>0.2779105600056937</v>
       </c>
     </row>
     <row r="16">
@@ -773,7 +773,7 @@
         <v>17071</v>
       </c>
       <c r="E16" t="n">
-        <v>0.173423485000967</v>
+        <v>0.2711487049964489</v>
       </c>
     </row>
     <row r="17">
@@ -794,7 +794,7 @@
         <v>2136</v>
       </c>
       <c r="E17" t="n">
-        <v>0.004217055000481196</v>
+        <v>0.00736568401043769</v>
       </c>
     </row>
     <row r="18">
@@ -815,7 +815,7 @@
         <v>692</v>
       </c>
       <c r="E18" t="n">
-        <v>0.002567946998169646</v>
+        <v>0.004415485993376933</v>
       </c>
     </row>
     <row r="19">
@@ -836,7 +836,7 @@
         <v>724</v>
       </c>
       <c r="E19" t="n">
-        <v>0.002929348993347958</v>
+        <v>0.005001676006941125</v>
       </c>
     </row>
     <row r="20">
@@ -857,7 +857,7 @@
         <v>775</v>
       </c>
       <c r="E20" t="n">
-        <v>0.003452531003858894</v>
+        <v>0.005535774995223619</v>
       </c>
     </row>
     <row r="21">
@@ -878,7 +878,7 @@
         <v>794</v>
       </c>
       <c r="E21" t="n">
-        <v>0.003682187998492736</v>
+        <v>0.005772446005721577</v>
       </c>
     </row>
     <row r="22">
@@ -899,7 +899,7 @@
         <v>49840</v>
       </c>
       <c r="E22" t="n">
-        <v>0.08219722800276941</v>
+        <v>0.1415659080084879</v>
       </c>
     </row>
     <row r="23">
@@ -920,7 +920,7 @@
         <v>7851</v>
       </c>
       <c r="E23" t="n">
-        <v>0.04459925500123063</v>
+        <v>0.06523129300330766</v>
       </c>
     </row>
     <row r="24">
@@ -941,7 +941,7 @@
         <v>4784</v>
       </c>
       <c r="E24" t="n">
-        <v>0.02536624899948947</v>
+        <v>0.03888741899572778</v>
       </c>
     </row>
     <row r="25">
@@ -962,7 +962,7 @@
         <v>8319</v>
       </c>
       <c r="E25" t="n">
-        <v>0.06241406800108962</v>
+        <v>0.08796854900720064</v>
       </c>
     </row>
     <row r="26">
@@ -983,7 +983,7 @@
         <v>4809</v>
       </c>
       <c r="E26" t="n">
-        <v>0.03140369700122392</v>
+        <v>0.0454000379977515</v>
       </c>
     </row>
     <row r="27">
@@ -1004,7 +1004,7 @@
         <v>124600</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1991850749982405</v>
+        <v>0.3342516929988051</v>
       </c>
     </row>
     <row r="28">
@@ -1025,7 +1025,7 @@
         <v>20525</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1985610080009792</v>
+        <v>0.3038843689864734</v>
       </c>
     </row>
     <row r="29">
@@ -1046,7 +1046,7 @@
         <v>19504</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1991506429985748</v>
+        <v>0.316666015991359</v>
       </c>
     </row>
     <row r="30">
@@ -1067,7 +1067,7 @@
         <v>20600</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2231662169942865</v>
+        <v>0.3439362789940787</v>
       </c>
     </row>
     <row r="31">
@@ -1088,7 +1088,7 @@
         <v>19578</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2136441269976785</v>
+        <v>0.3340900580078596</v>
       </c>
     </row>
     <row r="32">
@@ -1109,7 +1109,7 @@
         <v>2070000</v>
       </c>
       <c r="E32" t="n">
-        <v>3.625698049996572</v>
+        <v>6.546001648996025</v>
       </c>
     </row>
     <row r="33">
@@ -1130,7 +1130,7 @@
         <v>1369680</v>
       </c>
       <c r="E33" t="n">
-        <v>3.721459311003855</v>
+        <v>6.164249348003068</v>
       </c>
     </row>
     <row r="34">
@@ -1151,7 +1151,7 @@
         <v>1402847</v>
       </c>
       <c r="E34" t="n">
-        <v>4.167738889002067</v>
+        <v>6.941108212995459</v>
       </c>
     </row>
     <row r="35">
@@ -1172,7 +1172,7 @@
         <v>1605979</v>
       </c>
       <c r="E35" t="n">
-        <v>5.50981826500356</v>
+        <v>8.295261053004651</v>
       </c>
     </row>
     <row r="36">
@@ -1193,7 +1193,7 @@
         <v>1549714</v>
       </c>
       <c r="E36" t="n">
-        <v>5.514767667002161</v>
+        <v>8.304069053003332</v>
       </c>
     </row>
     <row r="37">
@@ -1214,7 +1214,7 @@
         <v>20000000</v>
       </c>
       <c r="E37" t="n">
-        <v>31.52742158600449</v>
+        <v>53.78559617900464</v>
       </c>
     </row>
     <row r="38">
@@ -1235,7 +1235,7 @@
         <v>2445462</v>
       </c>
       <c r="E38" t="n">
-        <v>12.79016619000322</v>
+        <v>16.87291693800944</v>
       </c>
     </row>
     <row r="39">
@@ -1256,7 +1256,7 @@
         <v>995678</v>
       </c>
       <c r="E39" t="n">
-        <v>8.458397934999084</v>
+        <v>11.89524010100286</v>
       </c>
     </row>
     <row r="40">
@@ -1277,7 +1277,7 @@
         <v>2567188</v>
       </c>
       <c r="E40" t="n">
-        <v>23.59077057499962</v>
+        <v>28.03955891799706</v>
       </c>
     </row>
     <row r="41">
@@ -1298,7 +1298,7 @@
         <v>712923</v>
       </c>
       <c r="E41" t="n">
-        <v>7.570853944998817</v>
+        <v>9.322999898009584</v>
       </c>
     </row>
     <row r="42">
@@ -1319,7 +1319,7 @@
         <v>83000000</v>
       </c>
       <c r="E42" t="n">
-        <v>128.6722444709958</v>
+        <v>217.7611038970063</v>
       </c>
     </row>
     <row r="43">
@@ -1340,7 +1340,7 @@
         <v>2734897</v>
       </c>
       <c r="E43" t="n">
-        <v>32.43403467199823</v>
+        <v>38.38030440399598</v>
       </c>
     </row>
     <row r="44">
@@ -1361,7 +1361,7 @@
         <v>1471694</v>
       </c>
       <c r="E44" t="n">
-        <v>19.53243472499889</v>
+        <v>25.96025929099414</v>
       </c>
     </row>
     <row r="45">
@@ -1382,7 +1382,7 @@
         <v>2718511</v>
       </c>
       <c r="E45" t="n">
-        <v>54.24646147800377</v>
+        <v>62.92718287500611</v>
       </c>
     </row>
     <row r="46">
@@ -1403,7 +1403,7 @@
         <v>1560019</v>
       </c>
       <c r="E46" t="n">
-        <v>28.83495225200022</v>
+        <v>33.84845888100972</v>
       </c>
     </row>
     <row r="47">
@@ -1424,7 +1424,7 @@
         <v>3690000</v>
       </c>
       <c r="E47" t="n">
-        <v>6.433731807992444</v>
+        <v>11.67326548800338</v>
       </c>
     </row>
     <row r="48">
@@ -1445,7 +1445,7 @@
         <v>2577393</v>
       </c>
       <c r="E48" t="n">
-        <v>6.76779491599882</v>
+        <v>11.33017684199149</v>
       </c>
     </row>
     <row r="49">
@@ -1466,7 +1466,7 @@
         <v>2367476</v>
       </c>
       <c r="E49" t="n">
-        <v>7.251122846995713</v>
+        <v>12.00220040499698</v>
       </c>
     </row>
     <row r="50">
@@ -1487,7 +1487,7 @@
         <v>2722276</v>
       </c>
       <c r="E50" t="n">
-        <v>9.189486382994801</v>
+        <v>14.11401870299596</v>
       </c>
     </row>
     <row r="51">
@@ -1508,7 +1508,7 @@
         <v>2420864</v>
       </c>
       <c r="E51" t="n">
-        <v>8.944107709001401</v>
+        <v>13.49605374099337</v>
       </c>
     </row>
     <row r="52">
@@ -1529,7 +1529,7 @@
         <v>16800000</v>
       </c>
       <c r="E52" t="n">
-        <v>26.43515767500503</v>
+        <v>45.40279168200505</v>
       </c>
     </row>
     <row r="53">
@@ -1550,7 +1550,7 @@
         <v>2305505</v>
       </c>
       <c r="E53" t="n">
-        <v>11.65422490199853</v>
+        <v>15.78876889799722</v>
       </c>
     </row>
     <row r="54">
@@ -1571,7 +1571,7 @@
         <v>1221798</v>
       </c>
       <c r="E54" t="n">
-        <v>8.644254487007856</v>
+        <v>12.22609734999423</v>
       </c>
     </row>
     <row r="55">
@@ -1592,7 +1592,7 @@
         <v>2479170</v>
       </c>
       <c r="E55" t="n">
-        <v>22.71688963199267</v>
+        <v>27.67630504899716</v>
       </c>
     </row>
     <row r="56">
@@ -1613,7 +1613,7 @@
         <v>1304855</v>
       </c>
       <c r="E56" t="n">
-        <v>14.8820648839901</v>
+        <v>18.08479998000257</v>
       </c>
     </row>
     <row r="57">
@@ -1634,7 +1634,7 @@
         <v>79500000</v>
       </c>
       <c r="E57" t="n">
-        <v>122.2881878550106</v>
+        <v>209.0494304309977</v>
       </c>
     </row>
     <row r="58">
@@ -1655,7 +1655,7 @@
         <v>3709462</v>
       </c>
       <c r="E58" t="n">
-        <v>40.5156517590076</v>
+        <v>49.21516536599665</v>
       </c>
     </row>
     <row r="59">
@@ -1676,7 +1676,7 @@
         <v>2590602</v>
       </c>
       <c r="E59" t="n">
-        <v>35.02543567500834</v>
+        <v>46.52588223299244</v>
       </c>
     </row>
     <row r="60">
@@ -1697,7 +1697,7 @@
         <v>3641446</v>
       </c>
       <c r="E60" t="n">
-        <v>76.65954678200069</v>
+        <v>87.71839000900218</v>
       </c>
     </row>
     <row r="61">
@@ -1718,7 +1718,7 @@
         <v>2658392</v>
       </c>
       <c r="E61" t="n">
-        <v>56.02694382199843</v>
+        <v>65.39027614500083</v>
       </c>
     </row>
   </sheetData>
@@ -1785,7 +1785,7 @@
         <v>120000</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2682985159990494</v>
+        <v>0.4342660840047756</v>
       </c>
     </row>
     <row r="3">
@@ -1806,7 +1806,7 @@
         <v>148332</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3719464620007784</v>
+        <v>0.6151491339987842</v>
       </c>
     </row>
     <row r="4">
@@ -1827,7 +1827,7 @@
         <v>89398</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2567091119999532</v>
+        <v>0.4391592110041529</v>
       </c>
     </row>
     <row r="5">
@@ -1848,7 +1848,7 @@
         <v>148577</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4515994890025468</v>
+        <v>0.7068641749938251</v>
       </c>
     </row>
     <row r="6">
@@ -1869,7 +1869,7 @@
         <v>89396</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3060872819987708</v>
+        <v>0.4790072169998894</v>
       </c>
     </row>
     <row r="7">
@@ -1890,7 +1890,7 @@
         <v>13800000</v>
       </c>
       <c r="E7" t="n">
-        <v>22.69400169299479</v>
+        <v>37.39261812900077</v>
       </c>
     </row>
     <row r="8">
@@ -1911,7 +1911,7 @@
         <v>7338918</v>
       </c>
       <c r="E8" t="n">
-        <v>24.84390040899598</v>
+        <v>35.25426222800161</v>
       </c>
     </row>
     <row r="9">
@@ -1932,7 +1932,7 @@
         <v>3683702</v>
       </c>
       <c r="E9" t="n">
-        <v>18.56450153500191</v>
+        <v>26.91546964700683</v>
       </c>
     </row>
     <row r="10">
@@ -1953,7 +1953,7 @@
         <v>7379733</v>
       </c>
       <c r="E10" t="n">
-        <v>39.12159483700088</v>
+        <v>49.25394255800347</v>
       </c>
     </row>
     <row r="11">
@@ -1974,7 +1974,7 @@
         <v>3681396</v>
       </c>
       <c r="E11" t="n">
-        <v>25.59362802399846</v>
+        <v>34.30945669599168</v>
       </c>
     </row>
     <row r="12">
@@ -1995,7 +1995,7 @@
         <v>53000000</v>
       </c>
       <c r="E12" t="n">
-        <v>82.13059319600143</v>
+        <v>140.7796935850056</v>
       </c>
     </row>
     <row r="13">
@@ -2016,7 +2016,7 @@
         <v>12840348</v>
       </c>
       <c r="E13" t="n">
-        <v>54.78684354299912</v>
+        <v>72.99056495100376</v>
       </c>
     </row>
     <row r="14">
@@ -2037,7 +2037,7 @@
         <v>4577270</v>
       </c>
       <c r="E14" t="n">
-        <v>24.83796236500348</v>
+        <v>34.555685653002</v>
       </c>
     </row>
     <row r="15">
@@ -2058,7 +2058,7 @@
         <v>12922220</v>
       </c>
       <c r="E15" t="n">
-        <v>81.11007291999704</v>
+        <v>104.8992867180059</v>
       </c>
     </row>
     <row r="16">
@@ -2079,7 +2079,7 @@
         <v>4585506</v>
       </c>
       <c r="E16" t="n">
-        <v>34.15631349700561</v>
+        <v>43.08881236200978</v>
       </c>
     </row>
     <row r="17">
@@ -2100,7 +2100,7 @@
         <v>90000</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2705890719953459</v>
+        <v>0.3835997210117057</v>
       </c>
     </row>
     <row r="18">
@@ -2121,7 +2121,7 @@
         <v>109459</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3657100569980685</v>
+        <v>0.530557594000129</v>
       </c>
     </row>
     <row r="19">
@@ -2142,7 +2142,7 @@
         <v>94459</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3428817160020117</v>
+        <v>0.5115735040017171</v>
       </c>
     </row>
     <row r="20">
@@ -2163,7 +2163,7 @@
         <v>109459</v>
       </c>
       <c r="E20" t="n">
-        <v>0.4084508669984643</v>
+        <v>0.5822852819983382</v>
       </c>
     </row>
     <row r="21">
@@ -2184,7 +2184,7 @@
         <v>94459</v>
       </c>
       <c r="E21" t="n">
-        <v>0.3937527009984478</v>
+        <v>0.5646136700088391</v>
       </c>
     </row>
     <row r="22">
@@ -2205,7 +2205,7 @@
         <v>6800000</v>
       </c>
       <c r="E22" t="n">
-        <v>11.34314738299872</v>
+        <v>18.74061004299438</v>
       </c>
     </row>
     <row r="23">
@@ -2226,7 +2226,7 @@
         <v>2879836</v>
       </c>
       <c r="E23" t="n">
-        <v>11.06419250400359</v>
+        <v>15.22049036099634</v>
       </c>
     </row>
     <row r="24">
@@ -2247,7 +2247,7 @@
         <v>1810008</v>
       </c>
       <c r="E24" t="n">
-        <v>10.48195680000208</v>
+        <v>14.97122426598798</v>
       </c>
     </row>
     <row r="25">
@@ -2268,7 +2268,7 @@
         <v>2879836</v>
       </c>
       <c r="E25" t="n">
-        <v>15.38272777300153</v>
+        <v>20.19500284499372</v>
       </c>
     </row>
     <row r="26">
@@ -2289,7 +2289,7 @@
         <v>1808146</v>
       </c>
       <c r="E26" t="n">
-        <v>13.74543755099876</v>
+        <v>17.82521583899506</v>
       </c>
     </row>
     <row r="27">
@@ -2310,7 +2310,7 @@
         <v>37000000</v>
       </c>
       <c r="E27" t="n">
-        <v>59.65257723099785</v>
+        <v>99.75754632000462</v>
       </c>
     </row>
     <row r="28">
@@ -2331,7 +2331,7 @@
         <v>4972604</v>
       </c>
       <c r="E28" t="n">
-        <v>27.16683422200003</v>
+        <v>34.89610663799976</v>
       </c>
     </row>
     <row r="29">
@@ -2352,7 +2352,7 @@
         <v>3296752</v>
       </c>
       <c r="E29" t="n">
-        <v>21.95632295700489</v>
+        <v>29.79970340800355</v>
       </c>
     </row>
     <row r="30">
@@ -2373,7 +2373,7 @@
         <v>4972604</v>
       </c>
       <c r="E30" t="n">
-        <v>38.11679077900044</v>
+        <v>49.33988917199895</v>
       </c>
     </row>
     <row r="31">
@@ -2394,7 +2394,7 @@
         <v>3296222</v>
       </c>
       <c r="E31" t="n">
-        <v>26.72337685200182</v>
+        <v>34.20889212700422</v>
       </c>
     </row>
     <row r="32">
@@ -2415,7 +2415,7 @@
         <v>90000</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9210556260004523</v>
+        <v>1.11903757500113</v>
       </c>
     </row>
     <row r="33">
@@ -2436,7 +2436,7 @@
         <v>84923</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9796162450002157</v>
+        <v>1.252294510006323</v>
       </c>
     </row>
     <row r="34">
@@ -2457,7 +2457,7 @@
         <v>84923</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9826084099986474</v>
+        <v>1.179804424013128</v>
       </c>
     </row>
     <row r="35">
@@ -2478,7 +2478,7 @@
         <v>84923</v>
       </c>
       <c r="E35" t="n">
-        <v>1.291304753001896</v>
+        <v>1.186803327000234</v>
       </c>
     </row>
     <row r="36">
@@ -2499,7 +2499,7 @@
         <v>84923</v>
       </c>
       <c r="E36" t="n">
-        <v>1.078869926001062</v>
+        <v>1.197759600006975</v>
       </c>
     </row>
     <row r="37">
@@ -2520,7 +2520,7 @@
         <v>6800000</v>
       </c>
       <c r="E37" t="n">
-        <v>12.85774857900105</v>
+        <v>22.33944455900928</v>
       </c>
     </row>
     <row r="38">
@@ -2541,7 +2541,7 @@
         <v>2934309</v>
       </c>
       <c r="E38" t="n">
-        <v>11.95205071999953</v>
+        <v>19.29329607699765</v>
       </c>
     </row>
     <row r="39">
@@ -2562,7 +2562,7 @@
         <v>1812148</v>
       </c>
       <c r="E39" t="n">
-        <v>8.595161565004673</v>
+        <v>14.09847174200695</v>
       </c>
     </row>
     <row r="40">
@@ -2583,7 +2583,7 @@
         <v>2934309</v>
       </c>
       <c r="E40" t="n">
-        <v>15.73497974700149</v>
+        <v>23.9155814639962</v>
       </c>
     </row>
     <row r="41">
@@ -2604,7 +2604,7 @@
         <v>1807916</v>
       </c>
       <c r="E41" t="n">
-        <v>10.92541129600431</v>
+        <v>16.03574053799093</v>
       </c>
     </row>
     <row r="42">
@@ -2625,7 +2625,7 @@
         <v>34000000</v>
       </c>
       <c r="E42" t="n">
-        <v>61.16180734999944</v>
+        <v>108.8301497609937</v>
       </c>
     </row>
     <row r="43">
@@ -2646,7 +2646,7 @@
         <v>7151322</v>
       </c>
       <c r="E43" t="n">
-        <v>41.0110633660006</v>
+        <v>60.61442365699622</v>
       </c>
     </row>
     <row r="44">
@@ -2667,7 +2667,7 @@
         <v>4236852</v>
       </c>
       <c r="E44" t="n">
-        <v>38.45806887099752</v>
+        <v>56.19837358299992</v>
       </c>
     </row>
     <row r="45">
@@ -2688,7 +2688,7 @@
         <v>7151322</v>
       </c>
       <c r="E45" t="n">
-        <v>54.65662452400284</v>
+        <v>79.34198274499795</v>
       </c>
     </row>
     <row r="46">
@@ -2709,7 +2709,7 @@
         <v>4214818</v>
       </c>
       <c r="E46" t="n">
-        <v>44.92725606800377</v>
+        <v>60.95489245699719</v>
       </c>
     </row>
     <row r="47">
@@ -2730,7 +2730,7 @@
         <v>840000</v>
       </c>
       <c r="E47" t="n">
-        <v>1.47853387700161</v>
+        <v>2.677357029999257</v>
       </c>
     </row>
     <row r="48">
@@ -2751,7 +2751,7 @@
         <v>879890</v>
       </c>
       <c r="E48" t="n">
-        <v>2.117933127010474</v>
+        <v>3.536816116000409</v>
       </c>
     </row>
     <row r="49">
@@ -2772,7 +2772,7 @@
         <v>874911</v>
       </c>
       <c r="E49" t="n">
-        <v>2.330293855004129</v>
+        <v>3.836212934009382</v>
       </c>
     </row>
     <row r="50">
@@ -2793,7 +2793,7 @@
         <v>882837</v>
       </c>
       <c r="E50" t="n">
-        <v>2.702914016001159</v>
+        <v>4.111728917996516</v>
       </c>
     </row>
     <row r="51">
@@ -2814,7 +2814,7 @@
         <v>877596</v>
       </c>
       <c r="E51" t="n">
-        <v>2.780574857009924</v>
+        <v>4.265971529006492</v>
       </c>
     </row>
     <row r="52">
@@ -2835,7 +2835,7 @@
         <v>6000000</v>
       </c>
       <c r="E52" t="n">
-        <v>9.504144099992118</v>
+        <v>16.28540998599783</v>
       </c>
     </row>
     <row r="53">
@@ -2856,7 +2856,7 @@
         <v>10330209</v>
       </c>
       <c r="E53" t="n">
-        <v>23.46875568499672</v>
+        <v>35.54263880700455</v>
       </c>
     </row>
     <row r="54">
@@ -2877,7 +2877,7 @@
         <v>2920537</v>
       </c>
       <c r="E54" t="n">
-        <v>7.889323527997476</v>
+        <v>11.87593407300301</v>
       </c>
     </row>
     <row r="55">
@@ -2898,7 +2898,7 @@
         <v>11052738</v>
       </c>
       <c r="E55" t="n">
-        <v>30.68521564100229</v>
+        <v>43.9188199229975</v>
       </c>
     </row>
     <row r="56">
@@ -2919,7 +2919,7 @@
         <v>3081199</v>
       </c>
       <c r="E56" t="n">
-        <v>9.229930214001797</v>
+        <v>13.09701940500236</v>
       </c>
     </row>
     <row r="57">
@@ -2940,7 +2940,7 @@
         <v>23500000</v>
       </c>
       <c r="E57" t="n">
-        <v>36.43146740799421</v>
+        <v>62.34008274899679</v>
       </c>
     </row>
     <row r="58">
@@ -2961,7 +2961,7 @@
         <v>11836355</v>
       </c>
       <c r="E58" t="n">
-        <v>31.36043068299477</v>
+        <v>46.07152797299204</v>
       </c>
     </row>
     <row r="59">
@@ -2982,7 +2982,7 @@
         <v>2541589</v>
       </c>
       <c r="E59" t="n">
-        <v>10.01124863600126</v>
+        <v>14.36279468800058</v>
       </c>
     </row>
     <row r="60">
@@ -3003,7 +3003,7 @@
         <v>20236336</v>
       </c>
       <c r="E60" t="n">
-        <v>59.77006085500761</v>
+        <v>86.04831000098784</v>
       </c>
     </row>
     <row r="61">
@@ -3024,7 +3024,7 @@
         <v>4391617</v>
       </c>
       <c r="E61" t="n">
-        <v>17.03169000300113</v>
+        <v>22.92530938600248</v>
       </c>
     </row>
     <row r="62">
@@ -3045,7 +3045,7 @@
         <v>1080000</v>
       </c>
       <c r="E62" t="n">
-        <v>2.015500535009778</v>
+        <v>3.583613772003446</v>
       </c>
     </row>
     <row r="63">
@@ -3066,7 +3066,7 @@
         <v>1110000</v>
       </c>
       <c r="E63" t="n">
-        <v>2.767837762992713</v>
+        <v>4.561874115999672</v>
       </c>
     </row>
     <row r="64">
@@ -3087,7 +3087,7 @@
         <v>1110000</v>
       </c>
       <c r="E64" t="n">
-        <v>3.048204680002527</v>
+        <v>5.024546314001782</v>
       </c>
     </row>
     <row r="65">
@@ -3108,7 +3108,7 @@
         <v>1110000</v>
       </c>
       <c r="E65" t="n">
-        <v>3.489153317001183</v>
+        <v>5.365207245995407</v>
       </c>
     </row>
     <row r="66">
@@ -3129,7 +3129,7 @@
         <v>1110000</v>
       </c>
       <c r="E66" t="n">
-        <v>3.635523675999139</v>
+        <v>5.57607519600424</v>
       </c>
     </row>
     <row r="67">
@@ -3150,7 +3150,7 @@
         <v>7900000</v>
       </c>
       <c r="E67" t="n">
-        <v>12.90621658600867</v>
+        <v>21.76227430999279</v>
       </c>
     </row>
     <row r="68">
@@ -3171,7 +3171,7 @@
         <v>3300000</v>
       </c>
       <c r="E68" t="n">
-        <v>7.472593055004836</v>
+        <v>11.36937612800102</v>
       </c>
     </row>
     <row r="69">
@@ -3192,7 +3192,7 @@
         <v>2521344</v>
       </c>
       <c r="E69" t="n">
-        <v>6.176656119001564</v>
+        <v>9.444409079995239</v>
       </c>
     </row>
     <row r="70">
@@ -3213,7 +3213,7 @@
         <v>3300000</v>
       </c>
       <c r="E70" t="n">
-        <v>9.148172245011665</v>
+        <v>13.306516851997</v>
       </c>
     </row>
     <row r="71">
@@ -3234,7 +3234,7 @@
         <v>2197780</v>
       </c>
       <c r="E71" t="n">
-        <v>6.684663812004146</v>
+        <v>9.430045143002644</v>
       </c>
     </row>
     <row r="72">
@@ -3255,7 +3255,7 @@
         <v>9000000</v>
       </c>
       <c r="E72" t="n">
-        <v>14.33975900900259</v>
+        <v>24.09288049700262</v>
       </c>
     </row>
     <row r="73">
@@ -3276,7 +3276,7 @@
         <v>7499766</v>
       </c>
       <c r="E73" t="n">
-        <v>16.60947763400327</v>
+        <v>25.20232958500856</v>
       </c>
     </row>
     <row r="74">
@@ -3297,7 +3297,7 @@
         <v>5728941</v>
       </c>
       <c r="E74" t="n">
-        <v>14.26723371300614</v>
+        <v>21.93620225100312</v>
       </c>
     </row>
     <row r="75">
@@ -3318,7 +3318,7 @@
         <v>7499786</v>
       </c>
       <c r="E75" t="n">
-        <v>20.07715436100261</v>
+        <v>29.49400094999874</v>
       </c>
     </row>
     <row r="76">
@@ -3339,7 +3339,7 @@
         <v>4524386</v>
       </c>
       <c r="E76" t="n">
-        <v>13.50076972600073</v>
+        <v>19.41906819101132</v>
       </c>
     </row>
     <row r="77">
@@ -3360,7 +3360,7 @@
         <v>525000</v>
       </c>
       <c r="E77" t="n">
-        <v>1.361939049995271</v>
+        <v>2.26145975801046</v>
       </c>
     </row>
     <row r="78">
@@ -3381,7 +3381,7 @@
         <v>645000</v>
       </c>
       <c r="E78" t="n">
-        <v>2.023746706006932</v>
+        <v>3.814742636997835</v>
       </c>
     </row>
     <row r="79">
@@ -3402,7 +3402,7 @@
         <v>645000</v>
       </c>
       <c r="E79" t="n">
-        <v>2.18201200698968</v>
+        <v>4.151694428990595</v>
       </c>
     </row>
     <row r="80">
@@ -3423,7 +3423,7 @@
         <v>645000</v>
       </c>
       <c r="E80" t="n">
-        <v>2.435108170000603</v>
+        <v>4.355832175991964</v>
       </c>
     </row>
     <row r="81">
@@ -3444,7 +3444,7 @@
         <v>645000</v>
       </c>
       <c r="E81" t="n">
-        <v>2.522327739992761</v>
+        <v>4.438339175991132</v>
       </c>
     </row>
     <row r="82">
@@ -3465,7 +3465,7 @@
         <v>3100000</v>
       </c>
       <c r="E82" t="n">
-        <v>5.685102400006144</v>
+        <v>10.12095094200049</v>
       </c>
     </row>
     <row r="83">
@@ -3486,7 +3486,7 @@
         <v>2200000</v>
       </c>
       <c r="E83" t="n">
-        <v>5.517453352993471</v>
+        <v>10.73493182400125</v>
       </c>
     </row>
     <row r="84">
@@ -3507,7 +3507,7 @@
         <v>2009427</v>
       </c>
       <c r="E84" t="n">
-        <v>5.400286649004556</v>
+        <v>10.31960234799772</v>
       </c>
     </row>
     <row r="85">
@@ -3528,7 +3528,7 @@
         <v>2200000</v>
       </c>
       <c r="E85" t="n">
-        <v>6.815596347005339</v>
+        <v>12.00344322899764</v>
       </c>
     </row>
     <row r="86">
@@ -3549,7 +3549,7 @@
         <v>1704140</v>
       </c>
       <c r="E86" t="n">
-        <v>5.578219893999631</v>
+        <v>9.669544940988999</v>
       </c>
     </row>
     <row r="87">
@@ -3570,7 +3570,7 @@
         <v>7000000</v>
       </c>
       <c r="E87" t="n">
-        <v>12.1889516129886</v>
+        <v>21.88447783500305</v>
       </c>
     </row>
     <row r="88">
@@ -3591,7 +3591,7 @@
         <v>6934999</v>
       </c>
       <c r="E88" t="n">
-        <v>16.52494321099948</v>
+        <v>32.28776554900105</v>
       </c>
     </row>
     <row r="89">
@@ -3612,7 +3612,7 @@
         <v>6357527</v>
       </c>
       <c r="E89" t="n">
-        <v>16.0716983799939</v>
+        <v>31.61455654499878</v>
       </c>
     </row>
     <row r="90">
@@ -3633,7 +3633,7 @@
         <v>6934999</v>
       </c>
       <c r="E90" t="n">
-        <v>19.15556146799645</v>
+        <v>35.67640119600401</v>
       </c>
     </row>
     <row r="91">
@@ -3654,7 +3654,7 @@
         <v>3860059</v>
       </c>
       <c r="E91" t="n">
-        <v>11.48711841800832</v>
+        <v>20.67004490000545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>